<commit_message>
Corrected and Verified code/1~3 for `SBS_set1` and `indel_set1`.
Note: Some p-values in "input/SBS_syn_data_distribution.pdf" and "input/indel_syn_data_distribution.pdf" has changed. Nevertheless other files have been successfully reproduced in the new destination directories.
</commit_message>
<xml_diff>
--- a/Code_Verification_Status.xlsx
+++ b/Code_Verification_Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD02770-9B28-4EC9-B162-6BF5C96F4618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8034991C-8632-41D0-91B2-21F39EEEC86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10515" yWindow="960" windowWidth="16350" windowHeight="13860" activeTab="1" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>Scripts that used to work in the old folder structure needs to be modified and verified, so that we can guarantee they can work under new folder structure . This file aims to record the progress of path-fixing and verification.</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Files to be deleted:</t>
-  </si>
-  <si>
-    <t>Files to be fixed:</t>
   </si>
   <si>
     <t>File deleted</t>
@@ -256,20 +253,81 @@
     <t>7_combine_extraction_metrics.R</t>
   </si>
   <si>
-    <t>8b_profiling_all.R</t>
-  </si>
-  <si>
     <t>9_plotting.R</t>
   </si>
   <si>
-    <t>8b_profiling_SP.py</t>
+    <t>8a_profiling_SP.py -&gt; 6a_profiling_SP.py</t>
+  </si>
+  <si>
+    <t>8b_profiling_all.R -&gt; 6b_profiling_all.R</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verified with SynSigGen v1.3.0 (removed dependencies of signature/exposure processing functions </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ICAMSxtra</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">;
+Replace these function dependencies with functions in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mSigTools</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Verified with SynSigGen v1.2.0 (by reproducing the same files)</t>
+  </si>
+  <si>
+    <t>Verified with SynSigGen v1.3.0</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>*: Some p-values in "input/SBS_syn_data_distribution.pdf" and "input/indel_syn_data_distribution.pdf" has changed, but other files have been successfully reproduced</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,8 +351,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +397,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,13 +428,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -365,9 +449,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -682,121 +774,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F851CE31-89F5-4788-B08D-CF7745DAE42C}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:13">
       <c r="B9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="3"/>
+    <row r="10" spans="1:13">
+      <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:13">
+      <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="6"/>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="30" customHeight="1">
+      <c r="A12" s="10"/>
+      <c r="B12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="5"/>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
-        <v>29</v>
+      <c r="B14" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:I5"/>
+    <mergeCell ref="B12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F44FBD-D5AF-4380-92CA-471632849700}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -816,121 +927,125 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3"/>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="10"/>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1">
+      <c r="B8" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30">
+      <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4"/>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B7" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>15</v>
@@ -941,44 +1056,75 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>39</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="8" t="s">
-        <v>40</v>
+      <c r="A22" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30">
+      <c r="A24" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A29" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -990,7 +1136,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1010,21 +1156,21 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3"/>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="4"/>
+      <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="6"/>
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1032,42 +1178,42 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1">
-      <c r="A10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
@@ -1097,27 +1243,27 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" customHeight="1">
+      <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1">
-      <c r="A16" s="8" t="s">
+    <row r="17" spans="1:5" ht="30" customHeight="1">
+      <c r="A17" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
-      <c r="A17" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A18" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
@@ -1126,22 +1272,22 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A23" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
More fixes to paths and comments of running and summarizing codes.
</commit_message>
<xml_diff>
--- a/Code_Verification_Status.xlsx
+++ b/Code_Verification_Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8034991C-8632-41D0-91B2-21F39EEEC86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A12DF8-61BA-4F57-80C0-25194C75C622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
+    <workbookView xWindow="14865" yWindow="1080" windowWidth="13050" windowHeight="13860" activeTab="1" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
   <si>
     <t>Scripts that used to work in the old folder structure needs to be modified and verified, so that we can guarantee they can work under new folder structure . This file aims to record the progress of path-fixing and verification.</t>
   </si>
@@ -224,15 +224,6 @@
   </si>
   <si>
     <t>indel</t>
-  </si>
-  <si>
-    <t>4b_run_mSigHdp.R</t>
-  </si>
-  <si>
-    <t>4c_run_mSigHdp.R</t>
-  </si>
-  <si>
-    <t>4d_run_mSigHdp.R</t>
   </si>
   <si>
     <t>4e_SBS_NR_hdp_gamma_beta_20.R</t>
@@ -321,6 +312,18 @@
   </si>
   <si>
     <t>*: Some p-values in "input/SBS_syn_data_distribution.pdf" and "input/indel_syn_data_distribution.pdf" has changed, but other files have been successfully reproduced</t>
+  </si>
+  <si>
+    <t>4c_run_signeR.R</t>
+  </si>
+  <si>
+    <t>4b_run_SignatureAnalyzer.R</t>
+  </si>
+  <si>
+    <t>4d_run_SP.py</t>
+  </si>
+  <si>
+    <t>Need to change branch to use as "master"</t>
   </si>
 </sst>
 </file>
@@ -450,6 +453,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -459,7 +463,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -783,61 +786,61 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
@@ -858,24 +861,24 @@
     <row r="11" spans="1:13">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
       <c r="A12" s="10"/>
-      <c r="B12" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
+      <c r="B12" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13">
@@ -906,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F44FBD-D5AF-4380-92CA-471632849700}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -935,13 +938,13 @@
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -953,14 +956,14 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1">
       <c r="A9" s="9"/>
@@ -990,11 +993,11 @@
       <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>46</v>
+      <c r="B11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1016,26 +1019,43 @@
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>31</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>32</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>33</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1045,7 +1065,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>15</v>
@@ -1053,43 +1073,45 @@
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30">
       <c r="A24" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30">
       <c r="A25" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1099,17 +1121,17 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1">
       <c r="A29" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1118,7 +1140,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1182,14 +1204,14 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1">
       <c r="A9" s="9"/>

</xml_diff>

<commit_message>
Corrected and verified data generation scripts for "SBS_set2" and "indel_set2"
1. Uploaded "common_code/data_gen_utils_2.R" for generation of data set 2. This file will be simplified and merged with "common_code/data_gen_utils.R" in future commits.

2. Updated version of SynSigGen to use as "1.2.0" - this version fixed the errors raised when generating one synthetic spectrum using one mutational signature.

3. Corrected the path and comments of data generation script for SBS_set2 and indel_set2. All data and plotting files have been reproduced. The exceptions are "XX_set2/XX_syn_data_distributions.pdf", where p-values in these figures were changed significantly.

This change may be an error fix or performance change due to upgrade of one or more dependency package(s). To be investigated in future commits.
</commit_message>
<xml_diff>
--- a/Code_Verification_Status.xlsx
+++ b/Code_Verification_Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943073DF-DC91-4B84-87F1-CC1AF7C833AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46380F9A-43D3-47F6-B20D-E1E0FD11B1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7995" yWindow="2910" windowWidth="13050" windowHeight="13860" activeTab="1" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
+    <workbookView xWindow="2115" yWindow="4455" windowWidth="13050" windowHeight="13860" activeTab="1" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>Scripts that used to work in the old folder structure needs to be modified and verified, so that we can guarantee they can work under new folder structure . This file aims to record the progress of path-fixing and verification.</t>
   </si>
@@ -321,6 +321,12 @@
   </si>
   <si>
     <t>4d_run_SP.py</t>
+  </si>
+  <si>
+    <t>Upgraded to v1.2.0-branch</t>
+  </si>
+  <si>
+    <t>For mSigHdp and hdpx, changed to use branch master. mSigHdp were now required to be &gt;=vXX and hdpx &gt;= vXX</t>
   </si>
 </sst>
 </file>
@@ -428,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -459,6 +465,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -904,10 +916,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F44FBD-D5AF-4380-92CA-471632849700}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -993,8 +1005,14 @@
       <c r="B11" s="11" t="s">
         <v>43</v>
       </c>
+      <c r="C11" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="D11" s="11" t="s">
         <v>43</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1002,24 +1020,29 @@
         <v>7</v>
       </c>
       <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="45" customHeight="1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
@@ -1092,59 +1115,54 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
+    <row r="22" spans="1:5" ht="30">
+      <c r="A22" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A23" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="7" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30">
-      <c r="A24" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30">
-      <c r="A25" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A29" s="9" t="s">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A27" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Chagnes for data generation utilitiy files in folder "common_code":
1. Retained functions which have identical codes in old files
- data_gen_utils.R
- data_gen_utils_2.R
in a new file
- data_gen_utils.R

2. Moved utility functions specially designed to generate data set 1 (9 cancer types, 3 noise levels) and data set 2 (18 cancer types, 2 noise levels) in two new files:
- data_gen_utils_set1.R
- data_gen_utils_set2.R
</commit_message>
<xml_diff>
--- a/Code_Verification_Status.xlsx
+++ b/Code_Verification_Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46380F9A-43D3-47F6-B20D-E1E0FD11B1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F8E42E-0511-4A46-B60D-8F7000E44E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="4455" windowWidth="13050" windowHeight="13860" activeTab="1" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
+    <workbookView xWindow="60" yWindow="1080" windowWidth="13050" windowHeight="13860" activeTab="1" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>Scripts that used to work in the old folder structure needs to be modified and verified, so that we can guarantee they can work under new folder structure . This file aims to record the progress of path-fixing and verification.</t>
   </si>
@@ -308,9 +308,6 @@
     <t>Verified with SynSigGen v1.3.0</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>*: Some p-values in "input/SBS_syn_data_distribution.pdf" and "input/indel_syn_data_distribution.pdf" has changed, but other files have been successfully reproduced</t>
   </si>
   <si>
@@ -323,10 +320,23 @@
     <t>4d_run_SP.py</t>
   </si>
   <si>
-    <t>Upgraded to v1.2.0-branch</t>
-  </si>
-  <si>
-    <t>For mSigHdp and hdpx, changed to use branch master. mSigHdp were now required to be &gt;=vXX and hdpx &gt;= vXX</t>
+    <r>
+      <t xml:space="preserve">Upgraded to v1.2.0-branch; all verified except </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>For mSigHdp and hdpx, changed to use branch master. mSigHdp were now required to be &gt;=v2.0.1.10 and hdpx &gt;= v1.0.3.9</t>
   </si>
 </sst>
 </file>
@@ -373,11 +383,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="20"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -456,7 +466,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -466,11 +475,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -795,61 +807,61 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
@@ -875,19 +887,19 @@
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
       <c r="A12" s="10"/>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13">
@@ -919,7 +931,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -965,14 +977,14 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1">
       <c r="A9" s="9"/>
@@ -998,25 +1010,19 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" ht="45" customHeight="1">
+      <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="B11" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="A12" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3"/>
@@ -1025,7 +1031,7 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="A13" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3"/>
@@ -1033,20 +1039,20 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="45" customHeight="1">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" ht="60" customHeight="1">
+      <c r="A14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
+      <c r="B14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>46</v>
+      <c r="A15" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1054,8 +1060,8 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>45</v>
+      <c r="A16" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1063,8 +1069,8 @@
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>47</v>
+      <c r="A17" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1072,7 +1078,7 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" t="s">
+      <c r="A18" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="2"/>
@@ -1085,7 +1091,7 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" t="s">
+      <c r="A19" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1098,7 +1104,7 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" t="s">
+      <c r="A20" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="2"/>
@@ -1107,7 +1113,7 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" t="s">
+      <c r="A21" s="15" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="2"/>
@@ -1116,12 +1122,12 @@
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="30">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="9"/>
@@ -1155,14 +1161,15 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1220,14 +1227,14 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1">
       <c r="A9" s="9"/>

</xml_diff>

<commit_message>
In each of 4 data set folders (SBS/indel set 1/2):
1. Removed "6_Summarize.R" and "7_combine_extraction_metrics.R", because the product of these two scripts - all_results.csv were included as a combined file under the top level directory - all_results_by_seed.csv

2. Before deletion, Wu Yang double checked the values between old all_results.csv under each data set folder, and new all_results_by_seed.csv. Wu Yang has verified that the old and new contents were identical.
</commit_message>
<xml_diff>
--- a/Code_Verification_Status.xlsx
+++ b/Code_Verification_Status.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F8E42E-0511-4A46-B60D-8F7000E44E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58905AAD-9538-40BD-81A4-3AD3E958FDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="1080" windowWidth="13050" windowHeight="13860" activeTab="1" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
+    <workbookView xWindow="14220" yWindow="1035" windowWidth="11925" windowHeight="13860" activeTab="2" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
-    <sheet name="XX" sheetId="3" r:id="rId2"/>
-    <sheet name="XX_down_samp" sheetId="2" r:id="rId3"/>
+    <sheet name="top_level" sheetId="4" r:id="rId2"/>
+    <sheet name="XX" sheetId="3" r:id="rId3"/>
+    <sheet name="XX_down_samp" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>Scripts that used to work in the old folder structure needs to be modified and verified, so that we can guarantee they can work under new folder structure . This file aims to record the progress of path-fixing and verification.</t>
   </si>
@@ -337,6 +338,21 @@
   </si>
   <si>
     <t>For mSigHdp and hdpx, changed to use branch master. mSigHdp were now required to be &gt;=v2.0.1.10 and hdpx &gt;= v1.0.3.9</t>
+  </si>
+  <si>
+    <t>Files to be fixed and verified (and renamed if applicable):</t>
+  </si>
+  <si>
+    <t>summarize_level1_dirs.R</t>
+  </si>
+  <si>
+    <t>Verified</t>
+  </si>
+  <si>
+    <t>Script file deleted, and the summary tables generated by old and new codes has been verified before file deletion.</t>
+  </si>
+  <si>
+    <t>Script file deleted</t>
   </si>
 </sst>
 </file>
@@ -444,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -467,6 +483,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -477,12 +502,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -801,67 +820,67 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
@@ -887,19 +906,19 @@
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
       <c r="A12" s="10"/>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13">
@@ -927,11 +946,102 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46671B95-6217-4B68-9FF4-38C904DEA3AC}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="10"/>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5"/>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:2" ht="30">
+      <c r="A11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="13"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="11"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="11"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A15" s="12"/>
+      <c r="B15" s="9"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F44FBD-D5AF-4380-92CA-471632849700}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -969,108 +1079,104 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B8" s="13" t="s">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1">
+      <c r="B10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="8" t="s">
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A11" s="9"/>
+      <c r="B11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="6" t="s">
+    <row r="12" spans="1:5" ht="30">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="45" customHeight="1">
-      <c r="A11" s="15" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="45" customHeight="1">
+      <c r="A13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B13" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="15" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="15" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" ht="60" customHeight="1">
-      <c r="A14" s="15" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" ht="60" customHeight="1">
+      <c r="A16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B16" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="15" t="s">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="15" t="s">
-        <v>46</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1078,105 +1184,147 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="15" t="s">
-        <v>31</v>
+      <c r="A18" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A19" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="15" t="s">
-        <v>33</v>
+      <c r="A20" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="30">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:5">
+      <c r="A22" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" ht="30">
+      <c r="A24" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A23" s="16" t="s">
+    <row r="25" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A25" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="7" t="s">
+      <c r="B27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A27" s="9" t="s">
+      <c r="B28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E6EB07-A541-434D-82DD-42B31E1EFA95}">
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -1227,14 +1375,14 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1">
       <c r="A9" s="9"/>

</xml_diff>

<commit_message>
In each of the 4 folders for results on "down-sampled" data sets (SBS/indel set 1/2):
1. Removed codes to:
- generate down-sampled data sets
- plot spectra in down-sampled data sets
as separate down-sampled data sets are no longer required by mSigHdp.

2. Added 1_copy_data_set.R to copy "Realistic" data set from folder of respective data set without down-sampling (e.g. SBS_set1 for SBS_set1_down_samp). This file is verified by Wu Yang so that it guarantees to copy all the contents without changes.
</commit_message>
<xml_diff>
--- a/Code_Verification_Status.xlsx
+++ b/Code_Verification_Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6909C23D-E8D3-45E2-9CFD-5033AA272EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915288A5-8D96-4D76-80F9-1E466A16B80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
+    <workbookView xWindow="3825" yWindow="2340" windowWidth="11925" windowHeight="13860" firstSheet="1" activeTab="3" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>Scripts that used to work in the old folder structure needs to be modified and verified, so that we can guarantee they can work under new folder structure . This file aims to record the progress of path-fixing and verification.</t>
   </si>
@@ -91,9 +91,6 @@
     <t>2_spectra_plot.R</t>
   </si>
   <si>
-    <t>3a_run_mSigHdp.R</t>
-  </si>
-  <si>
     <t>Files to be deleted:</t>
   </si>
   <si>
@@ -115,113 +112,7 @@
     <t>7a_profiling_SP.py</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">5_Summarize.R -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_Summarize.R</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">6_combine_extraction_metrics.R -&gt;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_combine_extraction_metrics.R</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">8_plotting.R -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_plotting.R</t>
-    </r>
-  </si>
-  <si>
     <t>Not applicable (The file is not included in the folder before, and nothing needs to be fixed)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">7b_profiling_all.R -&gt;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_profiling_all.R</t>
-    </r>
   </si>
   <si>
     <t>indel</t>
@@ -353,6 +244,101 @@
   </si>
   <si>
     <t>Script file deleted</t>
+  </si>
+  <si>
+    <t>3a_run_mSigHdp.R -&gt; 2a_run_mSigHdp.R</t>
+  </si>
+  <si>
+    <t>5_Summarize.R -&gt; 3_Summarize.R</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6_combine_extraction_metrics.R -&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_combine_extraction_metrics.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">7b_profiling_all.R -&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_profiling_all.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8_plotting.R -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_plotting.R</t>
+    </r>
+  </si>
+  <si>
+    <t>Files to be created:</t>
+  </si>
+  <si>
+    <t>1_copy_data_set.R</t>
+  </si>
+  <si>
+    <t>Fixed errors in path and comments, and created or renamed (if applicable)</t>
   </si>
 </sst>
 </file>
@@ -460,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -492,6 +478,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -504,7 +491,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -828,61 +818,61 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
@@ -903,30 +893,30 @@
     <row r="11" spans="1:13">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
       <c r="A12" s="10"/>
-      <c r="B12" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
+      <c r="B12" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="5"/>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -934,7 +924,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -974,25 +964,25 @@
     <row r="3" spans="1:2">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5"/>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1000,7 +990,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1">
@@ -1009,13 +999,13 @@
     </row>
     <row r="11" spans="1:2" ht="30">
       <c r="A11" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B12" s="13"/>
     </row>
@@ -1042,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F44FBD-D5AF-4380-92CA-471632849700}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1065,33 +1055,33 @@
     <row r="3" spans="1:5">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5"/>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1099,18 +1089,18 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1">
       <c r="A11" s="9"/>
@@ -1129,7 +1119,7 @@
     </row>
     <row r="12" spans="1:5" ht="30">
       <c r="A12" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1140,12 +1130,12 @@
       <c r="A13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="B13" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -1169,16 +1159,16 @@
       <c r="A16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="B16" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1187,7 +1177,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1196,7 +1186,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1205,7 +1195,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1218,7 +1208,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>15</v>
@@ -1231,7 +1221,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1240,7 +1230,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1249,7 +1239,7 @@
     </row>
     <row r="24" spans="1:5" ht="30">
       <c r="A24" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1258,7 +1248,7 @@
     </row>
     <row r="25" spans="1:5" ht="30.75" thickBot="1">
       <c r="A25" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -1267,63 +1257,63 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1">
       <c r="A29" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>51</v>
+        <v>32</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1340,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E6EB07-A541-434D-82DD-42B31E1EFA95}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1365,7 +1355,7 @@
     <row r="3" spans="1:5">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1377,7 +1367,7 @@
     <row r="5" spans="1:5">
       <c r="A5" s="5"/>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1385,18 +1375,18 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="17"/>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1">
       <c r="A9" s="9"/>
@@ -1413,59 +1403,63 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1">
-      <c r="A10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+    <row r="10" spans="1:5">
+      <c r="A10" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>17</v>
+      <c r="A11" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A12" s="9"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" customHeight="1">
+      <c r="A13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" customHeight="1">
+      <c r="A14" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1">
       <c r="A18" s="9" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1474,27 +1468,66 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>22</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A26" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Updates to Code_Verification_Status.xlsx to reflect changes in commit `94e966f`.
</commit_message>
<xml_diff>
--- a/Code_Verification_Status.xlsx
+++ b/Code_Verification_Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915288A5-8D96-4D76-80F9-1E466A16B80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF3301A-7FAE-41D7-BA58-F12CE612C5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="2340" windowWidth="11925" windowHeight="13860" firstSheet="1" activeTab="3" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
+    <workbookView xWindow="135" yWindow="405" windowWidth="11790" windowHeight="13860" firstSheet="1" activeTab="3" xr2:uid="{F468F767-8084-4786-9BF3-8BF7E9FFB5F6}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t>Scripts that used to work in the old folder structure needs to be modified and verified, so that we can guarantee they can work under new folder structure . This file aims to record the progress of path-fixing and verification.</t>
   </si>
@@ -246,12 +246,6 @@
     <t>Script file deleted</t>
   </si>
   <si>
-    <t>3a_run_mSigHdp.R -&gt; 2a_run_mSigHdp.R</t>
-  </si>
-  <si>
-    <t>5_Summarize.R -&gt; 3_Summarize.R</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">6_combine_extraction_metrics.R -&gt;
 </t>
@@ -280,33 +274,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">7b_profiling_all.R -&gt;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_profiling_all.R</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">8_plotting.R -&gt; </t>
     </r>
     <r>
@@ -339,6 +306,111 @@
   </si>
   <si>
     <t>Fixed errors in path and comments, and created or renamed (if applicable)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5_Summarize.R -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_Summarize.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3a_145879.sh -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_145879.sh</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3a_run_mSigHdp.R -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_run_mSigHdp.R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">7b_profiling_all.R -&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_profiling.R</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -446,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -490,10 +562,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1330,10 +1398,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E6EB07-A541-434D-82DD-42B31E1EFA95}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1355,7 +1423,7 @@
     <row r="3" spans="1:5">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1404,17 +1472,17 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="20" t="s">
-        <v>55</v>
+      <c r="A11" t="s">
+        <v>52</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1439,72 +1507,76 @@
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1">
       <c r="A14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1">
+      <c r="A17" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+    <row r="18" spans="1:5" ht="30" customHeight="1">
+      <c r="A18" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A19" s="9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" customHeight="1">
-      <c r="A17" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A18" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="D23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1513,21 +1585,30 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A26" s="9" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A27" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>